<commit_message>
figures ready, sums added
</commit_message>
<xml_diff>
--- a/output/tox_table.xlsx
+++ b/output/tox_table.xlsx
@@ -5,15 +5,24 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bryan\rscripts\esa2017\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bryan\rscripts\esa2017\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="tox_table" sheetId="1" r:id="rId1"/>
+    <sheet name="cyl" sheetId="3" r:id="rId1"/>
+    <sheet name="mic" sheetId="4" r:id="rId2"/>
+    <sheet name="sax" sheetId="2" r:id="rId3"/>
+    <sheet name="tox_table" sheetId="1" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">cyl!$A$2:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">mic!$A$2:$E$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">sax!$A$2:$E$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">tox_table!$A$2:$H$19</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -52,8 +61,110 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Milstead, William</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Milstead, William:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Milstead, William</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Milstead, William:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Milstead, William</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Milstead, William:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="28">
   <si>
     <t>genus</t>
   </si>
@@ -665,7 +776,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -699,6 +810,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1055,10 +1169,657 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>643</v>
+      </c>
+      <c r="C3" s="9">
+        <v>312</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3461</v>
+      </c>
+      <c r="E3" s="9">
+        <v>13539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>318</v>
+      </c>
+      <c r="C4" s="9">
+        <v>740</v>
+      </c>
+      <c r="D4" s="9">
+        <v>8527</v>
+      </c>
+      <c r="E4" s="9">
+        <v>25923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>47</v>
+      </c>
+      <c r="C5" s="9">
+        <v>438</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2481</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9">
+        <v>268</v>
+      </c>
+      <c r="C6" s="9">
+        <v>174</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1853</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9">
+        <v>134</v>
+      </c>
+      <c r="C7" s="9">
+        <v>74</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1328</v>
+      </c>
+      <c r="E7" s="9">
+        <v>7030</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>643</v>
+      </c>
+      <c r="C3" s="9">
+        <v>312</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3461</v>
+      </c>
+      <c r="E3" s="9">
+        <v>13539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9">
+        <v>137</v>
+      </c>
+      <c r="C4" s="9">
+        <v>188</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1170</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>397</v>
+      </c>
+      <c r="C5" s="9">
+        <v>110</v>
+      </c>
+      <c r="D5" s="9">
+        <v>13406</v>
+      </c>
+      <c r="E5" s="9">
+        <v>158052</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>166</v>
+      </c>
+      <c r="C6" s="9">
+        <v>891</v>
+      </c>
+      <c r="D6" s="9">
+        <v>6094</v>
+      </c>
+      <c r="E6" s="9">
+        <v>36273</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
+        <v>143</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1062</v>
+      </c>
+      <c r="D7" s="9">
+        <v>3271</v>
+      </c>
+      <c r="E7" s="9">
+        <v>8121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9">
+        <v>80</v>
+      </c>
+      <c r="C8" s="9">
+        <v>676</v>
+      </c>
+      <c r="D8" s="9">
+        <v>13383</v>
+      </c>
+      <c r="E8" s="9">
+        <v>51263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9">
+        <v>268</v>
+      </c>
+      <c r="C9" s="9">
+        <v>174</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1853</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5620</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9">
+        <v>661</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2953</v>
+      </c>
+      <c r="D10" s="9">
+        <v>27974</v>
+      </c>
+      <c r="E10" s="9">
+        <v>204147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="9">
+        <v>521</v>
+      </c>
+      <c r="C14" s="9">
+        <v>239</v>
+      </c>
+      <c r="D14" s="9">
+        <v>2929</v>
+      </c>
+      <c r="E14" s="9">
+        <v>14601</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="9">
+        <v>93</v>
+      </c>
+      <c r="C15" s="9">
+        <v>305</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1714</v>
+      </c>
+      <c r="E15" s="9">
+        <v>5530</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="9">
+        <v>106</v>
+      </c>
+      <c r="C16" s="9">
+        <v>323</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1802</v>
+      </c>
+      <c r="E16" s="9">
+        <v>6861</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="9">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9">
+        <v>703</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2030</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5357</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="9">
+        <v>283</v>
+      </c>
+      <c r="C18" s="9">
+        <v>201</v>
+      </c>
+      <c r="D18" s="9">
+        <v>407</v>
+      </c>
+      <c r="E18" s="9">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="9">
+        <v>187</v>
+      </c>
+      <c r="C19" s="9">
+        <v>490</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2421</v>
+      </c>
+      <c r="E19" s="9">
+        <v>8951</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C12:E12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>643</v>
+      </c>
+      <c r="C3" s="9">
+        <v>312</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3461</v>
+      </c>
+      <c r="E3" s="9">
+        <v>13539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>318</v>
+      </c>
+      <c r="C4" s="9">
+        <v>740</v>
+      </c>
+      <c r="D4" s="9">
+        <v>8527</v>
+      </c>
+      <c r="E4" s="9">
+        <v>25923</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>47</v>
+      </c>
+      <c r="C5" s="9">
+        <v>438</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2481</v>
+      </c>
+      <c r="E5" s="9">
+        <v>5268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="9">
+        <v>268</v>
+      </c>
+      <c r="C6" s="9">
+        <v>174</v>
+      </c>
+      <c r="D6" s="9">
+        <v>1853</v>
+      </c>
+      <c r="E6" s="9">
+        <v>5620</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="63" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="9">
+        <v>521</v>
+      </c>
+      <c r="C7" s="9">
+        <v>239</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2929</v>
+      </c>
+      <c r="E7" s="9">
+        <v>14601</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="9">
+        <v>93</v>
+      </c>
+      <c r="C8" s="9">
+        <v>305</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1714</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5530</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1078,16 +1839,16 @@
       <c r="B1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
     </row>
     <row r="2" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">

</xml_diff>